<commit_message>
Fucionalidades, logos e correçao de bugs
</commit_message>
<xml_diff>
--- a/Estoque.xlsx
+++ b/Estoque.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,15 +501,11 @@
           <t xml:space="preserve"> sedwe</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 21312312</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 12312</t>
-        </is>
+      <c r="E2" t="n">
+        <v>21312312</v>
+      </c>
+      <c r="F2" t="n">
+        <v>12312</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -518,6 +514,41 @@
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Lucia</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>22/09/2022</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>30/09/2022</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>12312</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>21312</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>12313</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>